<commit_message>
Added comments and more solutions.
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Faisal/Documents/Problems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FC50D7-C8C8-374E-8716-444756B3FCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D69D64-C44A-5B41-81E2-BE8DF523090A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -980,7 +992,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1095,8 +1107,44 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1178,6 +1226,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
@@ -1269,10 +1335,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1302,8 +1369,16 @@
     <xf numFmtId="0" fontId="15" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1522,8 +1597,8 @@
   </sheetPr>
   <dimension ref="A1:E1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1553,7 +1628,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1570,173 +1645,173 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:5" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="31" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:5" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:5" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:5" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="31" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:5" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:5" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:5" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:5" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:5" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:5" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="31" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1927,37 +2002,37 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+    <row r="25" spans="1:5" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="31" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
+    <row r="26" spans="1:5" s="34" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="31" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1996,7 +2071,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="29" t="s">
         <v>110</v>
       </c>
       <c r="B29" s="19" t="s">

</xml_diff>